<commit_message>
tim mak - fix duplicated sort and change getSort & getDatafunction
</commit_message>
<xml_diff>
--- a/pcmaker/Components.xlsx
+++ b/pcmaker/Components.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{70FC0B07-6677-4886-AA93-C912066153CA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8059ACB8-401C-4BE6-8933-E2E648E10870}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21630" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21660" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPU" sheetId="1" r:id="rId1"/>
@@ -24,16 +24,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Video Card'!$A$1:$I$101</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P20"/>
+  <oleSize ref="A85:N102"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3315,7 +3309,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>